<commit_message>
DE Préparation livrables rendu
</commit_message>
<xml_diff>
--- a/DE_Design-Event/04_DSS/281_Ecurie Piston Sport Auto_Spec Sheet.xlsx
+++ b/DE_Design-Event/04_DSS/281_Ecurie Piston Sport Auto_Spec Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin Niermaréchal\Documents\EPSA\02-Saison_Valkyriz\00-DirTech\02-Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin Niermaréchal\Documents\EPSA\03-GIT\Valkyriz\ELIZ-2021\DE_Design-Event\04_DSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C40A26-889D-4D4C-B256-DF01AD6DD53A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD85664-D7B4-4C80-93F5-17CD3A5EDCE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1525,7 +1525,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="334">
   <si>
     <t>Competitors: Please read the Instructions-Tips (tab below) prior to the completion and submission of this sheet.</t>
   </si>
@@ -2654,9 +2654,6 @@
     <t>2 driven wheels at the rear</t>
   </si>
   <si>
-    <t xml:space="preserve">331.25 </t>
-  </si>
-  <si>
     <t>230  for a few seconds</t>
   </si>
   <si>
@@ -2741,6 +2738,15 @@
   </si>
   <si>
     <t>3,7 / 8300</t>
+  </si>
+  <si>
+    <t>1,14:1</t>
+  </si>
+  <si>
+    <t>progressive</t>
+  </si>
+  <si>
+    <t>58,2</t>
   </si>
 </sst>
 </file>
@@ -3648,9 +3654,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3664,9 +3667,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3833,6 +3833,108 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3842,139 +3944,43 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4412,8 +4418,8 @@
   </sheetPr>
   <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94:H94"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85:H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4427,15 +4433,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
       <c r="H1" s="4">
         <v>2021</v>
       </c>
@@ -4443,169 +4449,169 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
       <c r="I2" s="8"/>
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="131">
+      <c r="B3" s="129"/>
+      <c r="C3" s="130">
         <v>281</v>
       </c>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="133"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="132"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" s="12" customFormat="1" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="128" t="s">
+      <c r="B4" s="136"/>
+      <c r="C4" s="137" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="130"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
+      <c r="A5" s="102"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="14">
         <v>2757</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="52" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="14">
         <v>1460</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="94">
+      <c r="H7" s="92">
         <v>1272</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="49" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="16">
         <v>1605</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="53" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="16">
         <v>1254</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="94">
+      <c r="H8" s="92">
         <v>1200</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="50" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="17">
         <v>290</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="98" t="s">
+      <c r="F9" s="133" t="s">
         <v>257</v>
       </c>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="50" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="17">
         <v>101.2</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="54" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="17">
         <v>128.80000000000001</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="54" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="18">
@@ -4613,118 +4619,118 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="53" t="s">
+      <c r="B11" s="48"/>
+      <c r="C11" s="51" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="19">
         <v>0.44</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="55" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="19">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
+      <c r="G11" s="134"/>
+      <c r="H11" s="134"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102" t="s">
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="134" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="122" t="s">
         <v>258</v>
       </c>
-      <c r="D14" s="135"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="134" t="s">
+      <c r="D14" s="123"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="122" t="s">
         <v>258</v>
       </c>
-      <c r="G14" s="135"/>
-      <c r="H14" s="106"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="124"/>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="134" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="122" t="s">
         <v>260</v>
       </c>
-      <c r="D15" s="135"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="134" t="s">
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="122" t="s">
         <v>261</v>
       </c>
-      <c r="G15" s="135"/>
-      <c r="H15" s="106"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="124"/>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="134" t="s">
+      <c r="B16" s="56"/>
+      <c r="C16" s="122" t="s">
         <v>259</v>
       </c>
-      <c r="D16" s="135"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="134" t="s">
+      <c r="D16" s="123"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="122" t="s">
         <v>262</v>
       </c>
-      <c r="G16" s="135"/>
-      <c r="H16" s="106"/>
+      <c r="G16" s="123"/>
+      <c r="H16" s="124"/>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="59" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="16">
         <v>25</v>
       </c>
-      <c r="E17" s="94">
+      <c r="E17" s="92">
         <v>25</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="49" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="16">
@@ -4735,249 +4741,269 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="56" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="20">
         <v>12.6</v>
       </c>
-      <c r="D18" s="136"/>
-      <c r="E18" s="137"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="126"/>
       <c r="F18" s="21">
         <v>15.8</v>
       </c>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="56" t="s">
         <v>202</v>
       </c>
       <c r="C19" s="20">
         <v>529</v>
       </c>
-      <c r="D19" s="105"/>
-      <c r="E19" s="105"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
       <c r="F19" s="21">
         <v>177</v>
       </c>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="56" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="20">
         <v>1.9187000000000001</v>
       </c>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="21">
         <v>1.8733</v>
       </c>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="108"/>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="55" t="s">
+      <c r="C21" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="55" t="s">
+      <c r="E21" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="G21" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="23"/>
+      <c r="H21" s="23" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="55" t="s">
+      <c r="C22" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="55" t="s">
+      <c r="E22" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="G22" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="23"/>
+      <c r="H22" s="23" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="22">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="D23" s="55" t="s">
+      <c r="C23" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="D23" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="G23" s="55" t="s">
+      <c r="E23" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="G23" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="23"/>
+      <c r="H23" s="23" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="56" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="22">
         <v>13.5</v>
       </c>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
       <c r="F24" s="24">
         <v>46</v>
       </c>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="108"/>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="56" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="22">
         <v>0.85</v>
       </c>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="108"/>
       <c r="F25" s="24">
         <v>0.51</v>
       </c>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
+      <c r="G25" s="108"/>
+      <c r="H25" s="108"/>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D26" s="105"/>
-      <c r="E26" s="105"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="108"/>
       <c r="F26" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
+      <c r="G26" s="108"/>
+      <c r="H26" s="108"/>
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
       <c r="F27" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
     </row>
     <row r="28" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="107" t="s">
+      <c r="B28" s="56"/>
+      <c r="C28" s="117" t="s">
         <v>265</v>
       </c>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="108" t="s">
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="121" t="s">
         <v>265</v>
       </c>
-      <c r="G28" s="108"/>
-      <c r="H28" s="108"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
     </row>
     <row r="29" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="56" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D29" s="105"/>
-      <c r="E29" s="105"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
       <c r="F29" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="G29" s="105"/>
-      <c r="H29" s="105"/>
+      <c r="G29" s="108"/>
+      <c r="H29" s="108"/>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="56" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="D30" s="105"/>
-      <c r="E30" s="105"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="108"/>
       <c r="F30" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="G30" s="105"/>
-      <c r="H30" s="105"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="108"/>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="60" t="s">
         <v>58</v>
       </c>
       <c r="D31" s="27" t="s">
@@ -4986,7 +5012,7 @@
       <c r="E31" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="F31" s="63" t="s">
+      <c r="F31" s="61" t="s">
         <v>59</v>
       </c>
       <c r="G31" s="29" t="s">
@@ -4997,211 +5023,217 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="66" t="s">
+      <c r="B32" s="56"/>
+      <c r="C32" s="64" t="s">
         <v>61</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>268</v>
       </c>
-      <c r="E32" s="68" t="s">
+      <c r="E32" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="64" t="s">
+      <c r="F32" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="G32" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="32"/>
+      <c r="H32" s="141" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="33" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="58"/>
-      <c r="C33" s="67" t="s">
+      <c r="B33" s="56"/>
+      <c r="C33" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="E33" s="69" t="s">
+      <c r="E33" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="33" t="s">
+      <c r="F33" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="G33" s="109"/>
-      <c r="H33" s="109"/>
+      <c r="G33" s="119"/>
+      <c r="H33" s="119"/>
     </row>
     <row r="34" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="D34" s="65" t="s">
+      <c r="D34" s="63" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="110"/>
+      <c r="F34" s="120"/>
+      <c r="G34" s="120"/>
+      <c r="H34" s="120"/>
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="107" t="s">
+      <c r="B35" s="57"/>
+      <c r="C35" s="117" t="s">
         <v>278</v>
       </c>
-      <c r="D35" s="107"/>
-      <c r="E35" s="107"/>
-      <c r="F35" s="107"/>
-      <c r="G35" s="107"/>
-      <c r="H35" s="107"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="117"/>
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="60"/>
-      <c r="C36" s="62" t="s">
+      <c r="B36" s="58"/>
+      <c r="C36" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="34" t="s">
         <v>279</v>
       </c>
-      <c r="E36" s="86" t="s">
+      <c r="E36" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="G36" s="70" t="s">
+      <c r="G36" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="H36" s="28"/>
+      <c r="H36" s="28" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="37" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="100"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="100"/>
-      <c r="G37" s="100"/>
-      <c r="H37" s="100"/>
+      <c r="A37" s="102"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
+      <c r="E37" s="102"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="102"/>
+      <c r="H37" s="102"/>
     </row>
     <row r="38" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="101" t="s">
+      <c r="C38" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101" t="s">
+      <c r="D38" s="118"/>
+      <c r="E38" s="118"/>
+      <c r="F38" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
+      <c r="G38" s="118"/>
+      <c r="H38" s="118"/>
     </row>
     <row r="39" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="111" t="s">
+      <c r="B39" s="69"/>
+      <c r="C39" s="101" t="s">
         <v>281</v>
       </c>
-      <c r="D39" s="111"/>
-      <c r="E39" s="111"/>
-      <c r="F39" s="111" t="s">
+      <c r="D39" s="101"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101" t="s">
         <v>282</v>
       </c>
-      <c r="G39" s="111"/>
-      <c r="H39" s="111"/>
+      <c r="G39" s="101"/>
+      <c r="H39" s="101"/>
     </row>
     <row r="40" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="71"/>
-      <c r="C40" s="111" t="s">
+      <c r="B40" s="69"/>
+      <c r="C40" s="101" t="s">
         <v>283</v>
       </c>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="111" t="s">
+      <c r="D40" s="101"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="101" t="s">
         <v>284</v>
       </c>
-      <c r="G40" s="111"/>
-      <c r="H40" s="111"/>
+      <c r="G40" s="101"/>
+      <c r="H40" s="101"/>
     </row>
     <row r="41" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="71"/>
-      <c r="C41" s="111" t="s">
+      <c r="B41" s="69"/>
+      <c r="C41" s="101" t="s">
         <v>285</v>
       </c>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="111" t="s">
+      <c r="D41" s="101"/>
+      <c r="E41" s="101"/>
+      <c r="F41" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="G41" s="111"/>
-      <c r="H41" s="111"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="101"/>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="71"/>
-      <c r="C42" s="111" t="s">
+      <c r="B42" s="69"/>
+      <c r="C42" s="101" t="s">
         <v>287</v>
       </c>
-      <c r="D42" s="111"/>
-      <c r="E42" s="111"/>
-      <c r="F42" s="111" t="s">
+      <c r="D42" s="101"/>
+      <c r="E42" s="101"/>
+      <c r="F42" s="101" t="s">
         <v>288</v>
       </c>
-      <c r="G42" s="111"/>
-      <c r="H42" s="111"/>
+      <c r="G42" s="101"/>
+      <c r="H42" s="101"/>
     </row>
     <row r="43" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="71"/>
-      <c r="C43" s="61" t="s">
+      <c r="B43" s="69"/>
+      <c r="C43" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="35">
         <v>3.38</v>
       </c>
-      <c r="E43" s="55" t="s">
+      <c r="E43" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F43" s="37">
+      <c r="F43" s="36">
         <v>2.27</v>
       </c>
-      <c r="G43" s="55" t="s">
+      <c r="G43" s="53" t="s">
         <v>82</v>
       </c>
       <c r="H43" s="23">
@@ -5209,421 +5241,421 @@
       </c>
     </row>
     <row r="44" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="72"/>
-      <c r="C44" s="111" t="s">
+      <c r="B44" s="70"/>
+      <c r="C44" s="101" t="s">
         <v>289</v>
       </c>
-      <c r="D44" s="111"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="111" t="s">
+      <c r="D44" s="101"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="101" t="s">
         <v>289</v>
       </c>
-      <c r="G44" s="111"/>
-      <c r="H44" s="111"/>
+      <c r="G44" s="101"/>
+      <c r="H44" s="101"/>
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="71"/>
-      <c r="C45" s="111" t="s">
+      <c r="B45" s="69"/>
+      <c r="C45" s="101" t="s">
         <v>290</v>
       </c>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111" t="s">
+      <c r="D45" s="101"/>
+      <c r="E45" s="101"/>
+      <c r="F45" s="101" t="s">
         <v>291</v>
       </c>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
+      <c r="G45" s="101"/>
+      <c r="H45" s="101"/>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="112" t="s">
+      <c r="B46" s="71"/>
+      <c r="C46" s="100" t="s">
         <v>292</v>
       </c>
-      <c r="D46" s="112"/>
-      <c r="E46" s="112"/>
-      <c r="F46" s="112" t="s">
+      <c r="D46" s="100"/>
+      <c r="E46" s="100"/>
+      <c r="F46" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="G46" s="112"/>
-      <c r="H46" s="112"/>
+      <c r="G46" s="100"/>
+      <c r="H46" s="100"/>
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="100"/>
-      <c r="B47" s="100"/>
-      <c r="C47" s="100"/>
-      <c r="D47" s="100"/>
-      <c r="E47" s="100"/>
-      <c r="F47" s="100"/>
-      <c r="G47" s="100"/>
-      <c r="H47" s="100"/>
+      <c r="A47" s="102"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="102"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="102"/>
+      <c r="F47" s="102"/>
+      <c r="G47" s="102"/>
+      <c r="H47" s="102"/>
     </row>
     <row r="48" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="74" t="s">
+      <c r="B48" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="113"/>
-      <c r="D48" s="113"/>
-      <c r="E48" s="113"/>
-      <c r="F48" s="113"/>
-      <c r="G48" s="113"/>
-      <c r="H48" s="113"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="99"/>
+      <c r="F48" s="99"/>
+      <c r="G48" s="99"/>
+      <c r="H48" s="99"/>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="111" t="s">
+      <c r="B49" s="73"/>
+      <c r="C49" s="101" t="s">
         <v>294</v>
       </c>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="111"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="101"/>
+      <c r="F49" s="101"/>
+      <c r="G49" s="101"/>
+      <c r="H49" s="101"/>
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="111" t="s">
+      <c r="B50" s="73"/>
+      <c r="C50" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
+      <c r="D50" s="101"/>
+      <c r="E50" s="101"/>
+      <c r="F50" s="101"/>
+      <c r="G50" s="101"/>
+      <c r="H50" s="101"/>
     </row>
     <row r="51" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="75"/>
-      <c r="C51" s="67" t="s">
+      <c r="B51" s="73"/>
+      <c r="C51" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="138">
+      <c r="D51" s="93">
         <v>270</v>
       </c>
-      <c r="E51" s="69" t="s">
+      <c r="E51" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="F51" s="139" t="s">
+      <c r="F51" s="114" t="s">
         <v>296</v>
       </c>
-      <c r="G51" s="140"/>
-      <c r="H51" s="141"/>
+      <c r="G51" s="115"/>
+      <c r="H51" s="116"/>
     </row>
     <row r="52" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="111" t="s">
+      <c r="B52" s="73"/>
+      <c r="C52" s="101" t="s">
         <v>297</v>
       </c>
-      <c r="D52" s="111"/>
-      <c r="E52" s="111"/>
-      <c r="F52" s="111"/>
-      <c r="G52" s="111"/>
-      <c r="H52" s="111"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="101"/>
+      <c r="F52" s="101"/>
+      <c r="G52" s="101"/>
+      <c r="H52" s="101"/>
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="B53" s="75"/>
-      <c r="C53" s="111" t="s">
+      <c r="B53" s="73"/>
+      <c r="C53" s="101" t="s">
         <v>297</v>
       </c>
-      <c r="D53" s="111"/>
-      <c r="E53" s="111"/>
-      <c r="F53" s="111"/>
-      <c r="G53" s="111"/>
-      <c r="H53" s="111"/>
+      <c r="D53" s="101"/>
+      <c r="E53" s="101"/>
+      <c r="F53" s="101"/>
+      <c r="G53" s="101"/>
+      <c r="H53" s="101"/>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="75"/>
-      <c r="C54" s="111" t="s">
+      <c r="B54" s="73"/>
+      <c r="C54" s="101" t="s">
         <v>298</v>
       </c>
-      <c r="D54" s="111"/>
-      <c r="E54" s="111"/>
-      <c r="F54" s="111"/>
-      <c r="G54" s="111"/>
-      <c r="H54" s="111"/>
+      <c r="D54" s="101"/>
+      <c r="E54" s="101"/>
+      <c r="F54" s="101"/>
+      <c r="G54" s="101"/>
+      <c r="H54" s="101"/>
     </row>
     <row r="55" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A55" s="76" t="s">
+      <c r="A55" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="B55" s="77"/>
-      <c r="C55" s="114" t="s">
+      <c r="B55" s="75"/>
+      <c r="C55" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="D55" s="114"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="114"/>
-      <c r="G55" s="114"/>
-      <c r="H55" s="114"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="112"/>
+      <c r="F55" s="112"/>
+      <c r="G55" s="112"/>
+      <c r="H55" s="112"/>
     </row>
     <row r="56" spans="1:8" s="2" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="115"/>
-      <c r="B56" s="115"/>
-      <c r="C56" s="115"/>
-      <c r="D56" s="115"/>
-      <c r="E56" s="115"/>
-      <c r="F56" s="115"/>
-      <c r="G56" s="115"/>
-      <c r="H56" s="115"/>
+      <c r="A56" s="113"/>
+      <c r="B56" s="113"/>
+      <c r="C56" s="113"/>
+      <c r="D56" s="113"/>
+      <c r="E56" s="113"/>
+      <c r="F56" s="113"/>
+      <c r="G56" s="113"/>
+      <c r="H56" s="113"/>
     </row>
     <row r="57" spans="1:8" s="2" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="116"/>
-      <c r="B57" s="116"/>
-      <c r="C57" s="116"/>
-      <c r="D57" s="116"/>
-      <c r="E57" s="116"/>
-      <c r="F57" s="116"/>
-      <c r="G57" s="116"/>
-      <c r="H57" s="116"/>
+      <c r="A57" s="111"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="111"/>
+      <c r="D57" s="111"/>
+      <c r="E57" s="111"/>
+      <c r="F57" s="111"/>
+      <c r="G57" s="111"/>
+      <c r="H57" s="111"/>
     </row>
     <row r="58" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="113"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="113"/>
-      <c r="F58" s="113"/>
-      <c r="G58" s="113"/>
-      <c r="H58" s="113"/>
+      <c r="C58" s="99"/>
+      <c r="D58" s="99"/>
+      <c r="E58" s="99"/>
+      <c r="F58" s="99"/>
+      <c r="G58" s="99"/>
+      <c r="H58" s="99"/>
     </row>
     <row r="59" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="78"/>
-      <c r="C59" s="111" t="s">
+      <c r="B59" s="76"/>
+      <c r="C59" s="101" t="s">
+        <v>326</v>
+      </c>
+      <c r="D59" s="101"/>
+      <c r="E59" s="101"/>
+      <c r="F59" s="101"/>
+      <c r="G59" s="101"/>
+      <c r="H59" s="101"/>
+    </row>
+    <row r="60" spans="1:8" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="76"/>
+      <c r="C60" s="94" t="s">
         <v>327</v>
       </c>
-      <c r="D59" s="111"/>
-      <c r="E59" s="111"/>
-      <c r="F59" s="111"/>
-      <c r="G59" s="111"/>
-      <c r="H59" s="111"/>
-    </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="78"/>
-      <c r="C60" s="118" t="s">
-        <v>328</v>
-      </c>
-      <c r="D60" s="119"/>
-      <c r="E60" s="119"/>
-      <c r="F60" s="119"/>
-      <c r="G60" s="119"/>
-      <c r="H60" s="120"/>
+      <c r="D60" s="97"/>
+      <c r="E60" s="97"/>
+      <c r="F60" s="97"/>
+      <c r="G60" s="97"/>
+      <c r="H60" s="98"/>
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A61" s="45" t="s">
+      <c r="A61" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="78"/>
-      <c r="C61" s="142" t="s">
+      <c r="B61" s="76"/>
+      <c r="C61" s="110" t="s">
+        <v>323</v>
+      </c>
+      <c r="D61" s="101"/>
+      <c r="E61" s="101"/>
+      <c r="F61" s="101"/>
+      <c r="G61" s="101"/>
+      <c r="H61" s="101"/>
+    </row>
+    <row r="62" spans="1:8" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="73"/>
+      <c r="C62" s="94" t="s">
+        <v>325</v>
+      </c>
+      <c r="D62" s="97"/>
+      <c r="E62" s="97"/>
+      <c r="F62" s="97"/>
+      <c r="G62" s="97"/>
+      <c r="H62" s="98"/>
+    </row>
+    <row r="63" spans="1:8" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" s="76"/>
+      <c r="C63" s="94" t="s">
+        <v>299</v>
+      </c>
+      <c r="D63" s="97"/>
+      <c r="E63" s="97"/>
+      <c r="F63" s="97"/>
+      <c r="G63" s="97"/>
+      <c r="H63" s="98"/>
+    </row>
+    <row r="64" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A64" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="76"/>
+      <c r="C64" s="101" t="s">
         <v>324</v>
       </c>
-      <c r="D61" s="111"/>
-      <c r="E61" s="111"/>
-      <c r="F61" s="111"/>
-      <c r="G61" s="111"/>
-      <c r="H61" s="111"/>
-    </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="75"/>
-      <c r="C62" s="118" t="s">
-        <v>326</v>
-      </c>
-      <c r="D62" s="119"/>
-      <c r="E62" s="119"/>
-      <c r="F62" s="119"/>
-      <c r="G62" s="119"/>
-      <c r="H62" s="120"/>
-    </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" s="78"/>
-      <c r="C63" s="118" t="s">
-        <v>299</v>
-      </c>
-      <c r="D63" s="119"/>
-      <c r="E63" s="119"/>
-      <c r="F63" s="119"/>
-      <c r="G63" s="119"/>
-      <c r="H63" s="120"/>
-    </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A64" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="B64" s="78"/>
-      <c r="C64" s="111" t="s">
-        <v>325</v>
-      </c>
-      <c r="D64" s="111"/>
-      <c r="E64" s="111"/>
-      <c r="F64" s="111"/>
-      <c r="G64" s="111"/>
-      <c r="H64" s="111"/>
+      <c r="D64" s="101"/>
+      <c r="E64" s="101"/>
+      <c r="F64" s="101"/>
+      <c r="G64" s="101"/>
+      <c r="H64" s="101"/>
     </row>
     <row r="65" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="B65" s="79"/>
-      <c r="C65" s="112" t="s">
+      <c r="B65" s="77"/>
+      <c r="C65" s="100" t="s">
         <v>257</v>
       </c>
-      <c r="D65" s="112"/>
-      <c r="E65" s="112"/>
-      <c r="F65" s="112"/>
-      <c r="G65" s="112"/>
-      <c r="H65" s="112"/>
+      <c r="D65" s="100"/>
+      <c r="E65" s="100"/>
+      <c r="F65" s="100"/>
+      <c r="G65" s="100"/>
+      <c r="H65" s="100"/>
     </row>
     <row r="66" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="100"/>
-      <c r="B66" s="100"/>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="100"/>
-      <c r="H66" s="100"/>
+      <c r="A66" s="102"/>
+      <c r="B66" s="102"/>
+      <c r="C66" s="102"/>
+      <c r="D66" s="102"/>
+      <c r="E66" s="102"/>
+      <c r="F66" s="102"/>
+      <c r="G66" s="102"/>
+      <c r="H66" s="102"/>
     </row>
     <row r="67" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="B67" s="44" t="s">
+      <c r="B67" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="113"/>
-      <c r="D67" s="113"/>
-      <c r="E67" s="113"/>
-      <c r="F67" s="113"/>
-      <c r="G67" s="113"/>
-      <c r="H67" s="113"/>
+      <c r="C67" s="99"/>
+      <c r="D67" s="99"/>
+      <c r="E67" s="99"/>
+      <c r="F67" s="99"/>
+      <c r="G67" s="99"/>
+      <c r="H67" s="99"/>
     </row>
     <row r="68" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A68" s="45" t="s">
+      <c r="A68" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="B68" s="83"/>
-      <c r="C68" s="111" t="s">
+      <c r="B68" s="81"/>
+      <c r="C68" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="D68" s="111"/>
-      <c r="E68" s="111"/>
-      <c r="F68" s="111"/>
-      <c r="G68" s="111"/>
-      <c r="H68" s="111"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="101"/>
+      <c r="H68" s="101"/>
     </row>
     <row r="69" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A69" s="45" t="s">
+      <c r="A69" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="B69" s="83"/>
-      <c r="C69" s="111" t="s">
+      <c r="B69" s="81"/>
+      <c r="C69" s="101" t="s">
         <v>301</v>
       </c>
-      <c r="D69" s="111"/>
-      <c r="E69" s="111"/>
-      <c r="F69" s="111"/>
-      <c r="G69" s="111"/>
-      <c r="H69" s="111"/>
+      <c r="D69" s="101"/>
+      <c r="E69" s="101"/>
+      <c r="F69" s="101"/>
+      <c r="G69" s="101"/>
+      <c r="H69" s="101"/>
     </row>
     <row r="70" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A70" s="45" t="s">
+      <c r="A70" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="B70" s="83"/>
-      <c r="C70" s="111" t="s">
+      <c r="B70" s="81"/>
+      <c r="C70" s="101" t="s">
         <v>302</v>
       </c>
-      <c r="D70" s="111"/>
-      <c r="E70" s="111"/>
-      <c r="F70" s="111"/>
-      <c r="G70" s="111"/>
-      <c r="H70" s="111"/>
+      <c r="D70" s="101"/>
+      <c r="E70" s="101"/>
+      <c r="F70" s="101"/>
+      <c r="G70" s="101"/>
+      <c r="H70" s="101"/>
     </row>
     <row r="71" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A71" s="45" t="s">
+      <c r="A71" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B71" s="83" t="s">
+      <c r="B71" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="C71" s="80" t="s">
+      <c r="C71" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="D71" s="37">
+      <c r="D71" s="36">
         <v>40</v>
       </c>
-      <c r="E71" s="54" t="s">
+      <c r="E71" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="F71" s="37" t="s">
+      <c r="F71" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="G71" s="105"/>
-      <c r="H71" s="105"/>
+      <c r="G71" s="108"/>
+      <c r="H71" s="108"/>
     </row>
     <row r="72" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A72" s="45" t="s">
+      <c r="A72" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="83" t="s">
+      <c r="B72" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="C72" s="61" t="s">
+      <c r="C72" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="D72" s="36">
+      <c r="D72" s="35">
         <v>4400</v>
       </c>
-      <c r="E72" s="55" t="s">
+      <c r="E72" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="F72" s="36" t="s">
+      <c r="F72" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="G72" s="55" t="s">
+      <c r="G72" s="53" t="s">
         <v>108</v>
       </c>
       <c r="H72" s="23" t="s">
@@ -5631,181 +5663,181 @@
       </c>
     </row>
     <row r="73" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A73" s="45" t="s">
+      <c r="A73" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B73" s="83"/>
-      <c r="C73" s="111" t="s">
+      <c r="B73" s="81"/>
+      <c r="C73" s="101" t="s">
         <v>257</v>
       </c>
-      <c r="D73" s="111"/>
-      <c r="E73" s="111"/>
-      <c r="F73" s="111"/>
-      <c r="G73" s="111"/>
-      <c r="H73" s="111"/>
+      <c r="D73" s="101"/>
+      <c r="E73" s="101"/>
+      <c r="F73" s="101"/>
+      <c r="G73" s="101"/>
+      <c r="H73" s="101"/>
     </row>
     <row r="74" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A74" s="45" t="s">
+      <c r="A74" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B74" s="83"/>
-      <c r="C74" s="111" t="s">
+      <c r="B74" s="81"/>
+      <c r="C74" s="101" t="s">
         <v>303</v>
       </c>
-      <c r="D74" s="111"/>
-      <c r="E74" s="111"/>
-      <c r="F74" s="111"/>
-      <c r="G74" s="111"/>
-      <c r="H74" s="111"/>
+      <c r="D74" s="101"/>
+      <c r="E74" s="101"/>
+      <c r="F74" s="101"/>
+      <c r="G74" s="101"/>
+      <c r="H74" s="101"/>
     </row>
     <row r="75" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A75" s="45" t="s">
+      <c r="A75" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B75" s="83" t="s">
+      <c r="B75" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C75" s="61" t="s">
+      <c r="C75" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="37">
+      <c r="D75" s="36">
         <v>356</v>
       </c>
-      <c r="E75" s="54" t="s">
+      <c r="E75" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F75" s="37">
+      <c r="F75" s="36">
         <v>305</v>
       </c>
-      <c r="G75" s="54" t="s">
+      <c r="G75" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="H75" s="38">
+      <c r="H75" s="142">
         <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A76" s="49" t="s">
+      <c r="A76" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="B76" s="84" t="s">
+      <c r="B76" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="C76" s="81" t="s">
+      <c r="C76" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="D76" s="39" t="s">
+      <c r="D76" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="E76" s="82" t="s">
+      <c r="E76" s="80" t="s">
         <v>119</v>
       </c>
-      <c r="F76" s="117" t="s">
+      <c r="F76" s="109" t="s">
         <v>257</v>
       </c>
-      <c r="G76" s="117"/>
-      <c r="H76" s="117"/>
+      <c r="G76" s="109"/>
+      <c r="H76" s="109"/>
     </row>
     <row r="77" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="100"/>
-      <c r="B77" s="100"/>
-      <c r="C77" s="100"/>
-      <c r="D77" s="100"/>
-      <c r="E77" s="100"/>
-      <c r="F77" s="100"/>
-      <c r="G77" s="100"/>
-      <c r="H77" s="100"/>
+      <c r="A77" s="102"/>
+      <c r="B77" s="102"/>
+      <c r="C77" s="102"/>
+      <c r="D77" s="102"/>
+      <c r="E77" s="102"/>
+      <c r="F77" s="102"/>
+      <c r="G77" s="102"/>
+      <c r="H77" s="102"/>
     </row>
     <row r="78" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A78" s="43" t="s">
+      <c r="A78" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="B78" s="44" t="s">
+      <c r="B78" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C78" s="121" t="s">
+      <c r="C78" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="D78" s="122"/>
-      <c r="E78" s="123"/>
-      <c r="F78" s="121" t="s">
+      <c r="D78" s="106"/>
+      <c r="E78" s="107"/>
+      <c r="F78" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="G78" s="122"/>
-      <c r="H78" s="123"/>
+      <c r="G78" s="106"/>
+      <c r="H78" s="107"/>
     </row>
     <row r="79" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A79" s="45" t="s">
+      <c r="A79" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="B79" s="83"/>
-      <c r="C79" s="118" t="s">
+      <c r="B79" s="81"/>
+      <c r="C79" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D79" s="119"/>
-      <c r="E79" s="120"/>
-      <c r="F79" s="118" t="s">
+      <c r="D79" s="97"/>
+      <c r="E79" s="98"/>
+      <c r="F79" s="94" t="s">
         <v>304</v>
       </c>
-      <c r="G79" s="119"/>
-      <c r="H79" s="120"/>
+      <c r="G79" s="97"/>
+      <c r="H79" s="98"/>
     </row>
     <row r="80" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A80" s="45" t="s">
+      <c r="A80" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="B80" s="83"/>
-      <c r="C80" s="118" t="s">
+      <c r="B80" s="81"/>
+      <c r="C80" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D80" s="119"/>
-      <c r="E80" s="120"/>
-      <c r="F80" s="118" t="s">
+      <c r="D80" s="97"/>
+      <c r="E80" s="98"/>
+      <c r="F80" s="94" t="s">
         <v>305</v>
       </c>
-      <c r="G80" s="119"/>
-      <c r="H80" s="120"/>
+      <c r="G80" s="97"/>
+      <c r="H80" s="98"/>
     </row>
     <row r="81" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A81" s="45" t="s">
+      <c r="A81" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="B81" s="83"/>
-      <c r="C81" s="118" t="s">
+      <c r="B81" s="81"/>
+      <c r="C81" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D81" s="119"/>
-      <c r="E81" s="120"/>
-      <c r="F81" s="118" t="s">
+      <c r="D81" s="97"/>
+      <c r="E81" s="98"/>
+      <c r="F81" s="94" t="s">
         <v>306</v>
       </c>
-      <c r="G81" s="119"/>
-      <c r="H81" s="120"/>
+      <c r="G81" s="97"/>
+      <c r="H81" s="98"/>
     </row>
     <row r="82" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A82" s="45" t="s">
+      <c r="A82" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="B82" s="83"/>
-      <c r="C82" s="118" t="s">
+      <c r="B82" s="81"/>
+      <c r="C82" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D82" s="119"/>
-      <c r="E82" s="120"/>
-      <c r="F82" s="118" t="s">
+      <c r="D82" s="97"/>
+      <c r="E82" s="98"/>
+      <c r="F82" s="94" t="s">
         <v>307</v>
       </c>
-      <c r="G82" s="119"/>
-      <c r="H82" s="120"/>
+      <c r="G82" s="97"/>
+      <c r="H82" s="98"/>
     </row>
     <row r="83" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A83" s="45" t="s">
+      <c r="A83" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="B83" s="83" t="s">
+      <c r="B83" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="C83" s="61" t="s">
+      <c r="C83" s="59" t="s">
         <v>200</v>
       </c>
       <c r="D83" s="16" t="s">
@@ -5814,502 +5846,502 @@
       <c r="E83" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="F83" s="51" t="s">
+      <c r="F83" s="49" t="s">
         <v>201</v>
       </c>
       <c r="G83" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="H83" s="15" t="s">
+      <c r="H83" s="15">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A84" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" s="81" t="s">
+        <v>120</v>
+      </c>
+      <c r="C84" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D84" s="97"/>
+      <c r="E84" s="98"/>
+      <c r="F84" s="94">
+        <v>5500</v>
+      </c>
+      <c r="G84" s="97"/>
+      <c r="H84" s="98"/>
+    </row>
+    <row r="85" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A85" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" s="81" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D85" s="97"/>
+      <c r="E85" s="98"/>
+      <c r="F85" s="94">
+        <v>4400</v>
+      </c>
+      <c r="G85" s="97"/>
+      <c r="H85" s="98"/>
+    </row>
+    <row r="86" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A86" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" s="81" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D86" s="97"/>
+      <c r="E86" s="98"/>
+      <c r="F86" s="94" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A84" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="B84" s="83" t="s">
-        <v>120</v>
-      </c>
-      <c r="C84" s="118" t="s">
+      <c r="G86" s="97"/>
+      <c r="H86" s="98"/>
+    </row>
+    <row r="87" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A87" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B87" s="81" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D84" s="119"/>
-      <c r="E84" s="120"/>
-      <c r="F84" s="118">
-        <v>5500</v>
-      </c>
-      <c r="G84" s="119"/>
-      <c r="H84" s="120"/>
-    </row>
-    <row r="85" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A85" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="B85" s="83" t="s">
-        <v>120</v>
-      </c>
-      <c r="C85" s="118" t="s">
+      <c r="D87" s="97"/>
+      <c r="E87" s="98"/>
+      <c r="F87" s="94">
+        <v>102</v>
+      </c>
+      <c r="G87" s="97"/>
+      <c r="H87" s="98"/>
+    </row>
+    <row r="88" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A88" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="81" t="s">
+        <v>192</v>
+      </c>
+      <c r="C88" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D85" s="119"/>
-      <c r="E85" s="120"/>
-      <c r="F85" s="118">
-        <v>4400</v>
-      </c>
-      <c r="G85" s="119"/>
-      <c r="H85" s="120"/>
-    </row>
-    <row r="86" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A86" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="B86" s="83" t="s">
-        <v>195</v>
-      </c>
-      <c r="C86" s="118" t="s">
+      <c r="D88" s="97"/>
+      <c r="E88" s="98"/>
+      <c r="F88" s="94" t="s">
+        <v>309</v>
+      </c>
+      <c r="G88" s="97"/>
+      <c r="H88" s="98"/>
+    </row>
+    <row r="89" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A89" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B89" s="81" t="s">
+        <v>191</v>
+      </c>
+      <c r="C89" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D86" s="119"/>
-      <c r="E86" s="120"/>
-      <c r="F86" s="118" t="s">
-        <v>309</v>
-      </c>
-      <c r="G86" s="119"/>
-      <c r="H86" s="120"/>
-    </row>
-    <row r="87" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A87" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="B87" s="83" t="s">
-        <v>164</v>
-      </c>
-      <c r="C87" s="118" t="s">
+      <c r="D89" s="97"/>
+      <c r="E89" s="98"/>
+      <c r="F89" s="94" t="s">
+        <v>310</v>
+      </c>
+      <c r="G89" s="97"/>
+      <c r="H89" s="98"/>
+    </row>
+    <row r="90" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A90" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B90" s="81"/>
+      <c r="C90" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D87" s="119"/>
-      <c r="E87" s="120"/>
-      <c r="F87" s="118">
-        <v>102</v>
-      </c>
-      <c r="G87" s="119"/>
-      <c r="H87" s="120"/>
-    </row>
-    <row r="88" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A88" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="B88" s="83" t="s">
-        <v>192</v>
-      </c>
-      <c r="C88" s="118" t="s">
+      <c r="D90" s="97"/>
+      <c r="E90" s="98"/>
+      <c r="F90" s="94" t="s">
+        <v>311</v>
+      </c>
+      <c r="G90" s="97"/>
+      <c r="H90" s="98"/>
+    </row>
+    <row r="91" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A91" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B91" s="81"/>
+      <c r="C91" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D88" s="119"/>
-      <c r="E88" s="120"/>
-      <c r="F88" s="118" t="s">
-        <v>310</v>
-      </c>
-      <c r="G88" s="119"/>
-      <c r="H88" s="120"/>
-    </row>
-    <row r="89" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A89" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="B89" s="83" t="s">
-        <v>191</v>
-      </c>
-      <c r="C89" s="118" t="s">
+      <c r="D91" s="97"/>
+      <c r="E91" s="98"/>
+      <c r="F91" s="94" t="s">
+        <v>277</v>
+      </c>
+      <c r="G91" s="97"/>
+      <c r="H91" s="98"/>
+    </row>
+    <row r="92" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A92" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B92" s="81"/>
+      <c r="C92" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D89" s="119"/>
-      <c r="E89" s="120"/>
-      <c r="F89" s="118" t="s">
-        <v>311</v>
-      </c>
-      <c r="G89" s="119"/>
-      <c r="H89" s="120"/>
-    </row>
-    <row r="90" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A90" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="B90" s="83"/>
-      <c r="C90" s="118" t="s">
+      <c r="D92" s="97"/>
+      <c r="E92" s="98"/>
+      <c r="F92" s="94" t="s">
+        <v>312</v>
+      </c>
+      <c r="G92" s="97"/>
+      <c r="H92" s="98"/>
+    </row>
+    <row r="93" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A93" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="B93" s="81" t="s">
+        <v>194</v>
+      </c>
+      <c r="C93" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D90" s="119"/>
-      <c r="E90" s="120"/>
-      <c r="F90" s="118" t="s">
-        <v>312</v>
-      </c>
-      <c r="G90" s="119"/>
-      <c r="H90" s="120"/>
-    </row>
-    <row r="91" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A91" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="B91" s="83"/>
-      <c r="C91" s="118" t="s">
+      <c r="D93" s="97"/>
+      <c r="E93" s="98"/>
+      <c r="F93" s="94" t="s">
+        <v>313</v>
+      </c>
+      <c r="G93" s="97"/>
+      <c r="H93" s="98"/>
+    </row>
+    <row r="94" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A94" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B94" s="81" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D91" s="119"/>
-      <c r="E91" s="120"/>
-      <c r="F91" s="118" t="s">
-        <v>277</v>
-      </c>
-      <c r="G91" s="119"/>
-      <c r="H91" s="120"/>
-    </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A92" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="B92" s="83"/>
-      <c r="C92" s="118" t="s">
+      <c r="D94" s="97"/>
+      <c r="E94" s="98"/>
+      <c r="F94" s="94">
+        <v>90</v>
+      </c>
+      <c r="G94" s="97"/>
+      <c r="H94" s="98"/>
+    </row>
+    <row r="95" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A95" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" s="81"/>
+      <c r="C95" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D92" s="119"/>
-      <c r="E92" s="120"/>
-      <c r="F92" s="118" t="s">
-        <v>313</v>
-      </c>
-      <c r="G92" s="119"/>
-      <c r="H92" s="120"/>
-    </row>
-    <row r="93" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A93" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="B93" s="83" t="s">
+      <c r="D95" s="97"/>
+      <c r="E95" s="98"/>
+      <c r="F95" s="94" t="s">
+        <v>318</v>
+      </c>
+      <c r="G95" s="97"/>
+      <c r="H95" s="98"/>
+    </row>
+    <row r="96" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A96" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B96" s="81" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D96" s="97"/>
+      <c r="E96" s="98"/>
+      <c r="F96" s="94" t="s">
+        <v>330</v>
+      </c>
+      <c r="G96" s="97"/>
+      <c r="H96" s="98"/>
+    </row>
+    <row r="97" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A97" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B97" s="81" t="s">
+        <v>178</v>
+      </c>
+      <c r="C97" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D97" s="95"/>
+      <c r="E97" s="96"/>
+      <c r="F97" s="94">
+        <v>504</v>
+      </c>
+      <c r="G97" s="95"/>
+      <c r="H97" s="96"/>
+    </row>
+    <row r="98" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A98" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="B98" s="81"/>
+      <c r="C98" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D98" s="97"/>
+      <c r="E98" s="98"/>
+      <c r="F98" s="94" t="s">
+        <v>314</v>
+      </c>
+      <c r="G98" s="97"/>
+      <c r="H98" s="98"/>
+    </row>
+    <row r="99" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A99" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B99" s="81"/>
+      <c r="C99" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D99" s="97"/>
+      <c r="E99" s="98"/>
+      <c r="F99" s="94" t="s">
+        <v>315</v>
+      </c>
+      <c r="G99" s="97"/>
+      <c r="H99" s="98"/>
+    </row>
+    <row r="100" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A100" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B100" s="81" t="s">
         <v>194</v>
       </c>
-      <c r="C93" s="118" t="s">
+      <c r="C100" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D93" s="119"/>
-      <c r="E93" s="120"/>
-      <c r="F93" s="118" t="s">
-        <v>314</v>
-      </c>
-      <c r="G93" s="119"/>
-      <c r="H93" s="120"/>
-    </row>
-    <row r="94" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A94" s="45" t="s">
-        <v>196</v>
-      </c>
-      <c r="B94" s="83" t="s">
+      <c r="D100" s="97"/>
+      <c r="E100" s="98"/>
+      <c r="F100" s="94" t="s">
+        <v>316</v>
+      </c>
+      <c r="G100" s="97"/>
+      <c r="H100" s="98"/>
+    </row>
+    <row r="101" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A101" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B101" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="C94" s="118" t="s">
+      <c r="C101" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D94" s="119"/>
-      <c r="E94" s="120"/>
-      <c r="F94" s="118">
-        <v>90</v>
-      </c>
-      <c r="G94" s="119"/>
-      <c r="H94" s="120"/>
-    </row>
-    <row r="95" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A95" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="B95" s="83"/>
-      <c r="C95" s="118" t="s">
+      <c r="D101" s="97"/>
+      <c r="E101" s="98"/>
+      <c r="F101" s="94">
+        <v>55.5</v>
+      </c>
+      <c r="G101" s="97"/>
+      <c r="H101" s="98"/>
+    </row>
+    <row r="102" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A102" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B102" s="81" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="D95" s="119"/>
-      <c r="E95" s="120"/>
-      <c r="F95" s="118" t="s">
+      <c r="D102" s="97"/>
+      <c r="E102" s="98"/>
+      <c r="F102" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="G102" s="97"/>
+      <c r="H102" s="98"/>
+    </row>
+    <row r="103" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A103" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="B103" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D103" s="97"/>
+      <c r="E103" s="98"/>
+      <c r="F103" s="94" t="s">
+        <v>317</v>
+      </c>
+      <c r="G103" s="97"/>
+      <c r="H103" s="98"/>
+    </row>
+    <row r="104" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A104" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="B104" s="81" t="s">
+        <v>183</v>
+      </c>
+      <c r="C104" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D104" s="97"/>
+      <c r="E104" s="98"/>
+      <c r="F104" s="94">
+        <v>44258</v>
+      </c>
+      <c r="G104" s="97"/>
+      <c r="H104" s="98"/>
+    </row>
+    <row r="105" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A105" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="B105" s="81"/>
+      <c r="C105" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D105" s="97"/>
+      <c r="E105" s="98"/>
+      <c r="F105" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="G105" s="97"/>
+      <c r="H105" s="98"/>
+    </row>
+    <row r="106" spans="1:8" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="B106" s="82"/>
+      <c r="C106" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D106" s="97"/>
+      <c r="E106" s="98"/>
+      <c r="F106" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="G106" s="97"/>
+      <c r="H106" s="98"/>
+    </row>
+    <row r="107" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="102"/>
+      <c r="B107" s="102"/>
+      <c r="C107" s="102"/>
+      <c r="D107" s="102"/>
+      <c r="E107" s="102"/>
+      <c r="F107" s="102"/>
+      <c r="G107" s="102"/>
+      <c r="H107" s="102"/>
+    </row>
+    <row r="108" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B108" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" s="99"/>
+      <c r="D108" s="99"/>
+      <c r="E108" s="99"/>
+      <c r="F108" s="99"/>
+      <c r="G108" s="99"/>
+      <c r="H108" s="99"/>
+    </row>
+    <row r="109" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A109" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B109" s="81"/>
+      <c r="C109" s="101" t="s">
+        <v>329</v>
+      </c>
+      <c r="D109" s="101"/>
+      <c r="E109" s="101"/>
+      <c r="F109" s="101"/>
+      <c r="G109" s="101"/>
+      <c r="H109" s="101"/>
+    </row>
+    <row r="110" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A110" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="B110" s="81"/>
+      <c r="C110" s="101" t="s">
         <v>319</v>
       </c>
-      <c r="G95" s="119"/>
-      <c r="H95" s="120"/>
-    </row>
-    <row r="96" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A96" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="B96" s="83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C96" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D96" s="119"/>
-      <c r="E96" s="120"/>
-      <c r="F96" s="118" t="s">
-        <v>331</v>
-      </c>
-      <c r="G96" s="119"/>
-      <c r="H96" s="120"/>
-    </row>
-    <row r="97" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A97" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="B97" s="83" t="s">
-        <v>178</v>
-      </c>
-      <c r="C97" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D97" s="126"/>
-      <c r="E97" s="127"/>
-      <c r="F97" s="118">
-        <v>504</v>
-      </c>
-      <c r="G97" s="126"/>
-      <c r="H97" s="127"/>
-    </row>
-    <row r="98" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A98" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="B98" s="83"/>
-      <c r="C98" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D98" s="119"/>
-      <c r="E98" s="120"/>
-      <c r="F98" s="118" t="s">
-        <v>315</v>
-      </c>
-      <c r="G98" s="119"/>
-      <c r="H98" s="120"/>
-    </row>
-    <row r="99" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A99" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="B99" s="83"/>
-      <c r="C99" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D99" s="119"/>
-      <c r="E99" s="120"/>
-      <c r="F99" s="118" t="s">
-        <v>316</v>
-      </c>
-      <c r="G99" s="119"/>
-      <c r="H99" s="120"/>
-    </row>
-    <row r="100" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A100" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="B100" s="83" t="s">
-        <v>194</v>
-      </c>
-      <c r="C100" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D100" s="119"/>
-      <c r="E100" s="120"/>
-      <c r="F100" s="118" t="s">
-        <v>317</v>
-      </c>
-      <c r="G100" s="119"/>
-      <c r="H100" s="120"/>
-    </row>
-    <row r="101" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A101" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="B101" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="C101" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D101" s="119"/>
-      <c r="E101" s="120"/>
-      <c r="F101" s="118">
-        <v>55.5</v>
-      </c>
-      <c r="G101" s="119"/>
-      <c r="H101" s="120"/>
-    </row>
-    <row r="102" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A102" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="B102" s="83" t="s">
-        <v>179</v>
-      </c>
-      <c r="C102" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D102" s="119"/>
-      <c r="E102" s="120"/>
-      <c r="F102" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="G102" s="119"/>
-      <c r="H102" s="120"/>
-    </row>
-    <row r="103" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A103" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="B103" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="C103" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D103" s="119"/>
-      <c r="E103" s="120"/>
-      <c r="F103" s="118" t="s">
-        <v>318</v>
-      </c>
-      <c r="G103" s="119"/>
-      <c r="H103" s="120"/>
-    </row>
-    <row r="104" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A104" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="B104" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="C104" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D104" s="119"/>
-      <c r="E104" s="120"/>
-      <c r="F104" s="118">
-        <v>44258</v>
-      </c>
-      <c r="G104" s="119"/>
-      <c r="H104" s="120"/>
-    </row>
-    <row r="105" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A105" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="B105" s="83"/>
-      <c r="C105" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D105" s="119"/>
-      <c r="E105" s="120"/>
-      <c r="F105" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="G105" s="119"/>
-      <c r="H105" s="120"/>
-    </row>
-    <row r="106" spans="1:8" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="B106" s="84"/>
-      <c r="C106" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="D106" s="119"/>
-      <c r="E106" s="120"/>
-      <c r="F106" s="118" t="s">
-        <v>257</v>
-      </c>
-      <c r="G106" s="119"/>
-      <c r="H106" s="120"/>
-    </row>
-    <row r="107" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="100"/>
-      <c r="B107" s="100"/>
-      <c r="C107" s="100"/>
-      <c r="D107" s="100"/>
-      <c r="E107" s="100"/>
-      <c r="F107" s="100"/>
-      <c r="G107" s="100"/>
-      <c r="H107" s="100"/>
-    </row>
-    <row r="108" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="B108" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C108" s="113"/>
-      <c r="D108" s="113"/>
-      <c r="E108" s="113"/>
-      <c r="F108" s="113"/>
-      <c r="G108" s="113"/>
-      <c r="H108" s="113"/>
-    </row>
-    <row r="109" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A109" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="B109" s="83"/>
-      <c r="C109" s="111" t="s">
-        <v>330</v>
-      </c>
-      <c r="D109" s="111"/>
-      <c r="E109" s="111"/>
-      <c r="F109" s="111"/>
-      <c r="G109" s="111"/>
-      <c r="H109" s="111"/>
-    </row>
-    <row r="110" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A110" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="B110" s="83"/>
-      <c r="C110" s="111" t="s">
+      <c r="D110" s="101"/>
+      <c r="E110" s="101"/>
+      <c r="F110" s="101"/>
+      <c r="G110" s="101"/>
+      <c r="H110" s="101"/>
+    </row>
+    <row r="111" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A111" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="B111" s="81" t="s">
+        <v>123</v>
+      </c>
+      <c r="C111" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="D110" s="111"/>
-      <c r="E110" s="111"/>
-      <c r="F110" s="111"/>
-      <c r="G110" s="111"/>
-      <c r="H110" s="111"/>
-    </row>
-    <row r="111" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A111" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="B111" s="83" t="s">
-        <v>123</v>
-      </c>
-      <c r="C111" s="25" t="s">
-        <v>321</v>
-      </c>
-      <c r="D111" s="124"/>
-      <c r="E111" s="124"/>
-      <c r="F111" s="124"/>
-      <c r="G111" s="124"/>
-      <c r="H111" s="124"/>
+      <c r="D111" s="103"/>
+      <c r="E111" s="103"/>
+      <c r="F111" s="103"/>
+      <c r="G111" s="103"/>
+      <c r="H111" s="103"/>
     </row>
     <row r="112" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A112" s="45" t="s">
+      <c r="A112" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B112" s="83" t="s">
+      <c r="B112" s="81" t="s">
         <v>125</v>
       </c>
-      <c r="C112" s="61" t="s">
+      <c r="C112" s="59" t="s">
         <v>126</v>
       </c>
       <c r="D112" s="14">
         <v>151</v>
       </c>
-      <c r="E112" s="54" t="s">
+      <c r="E112" s="52" t="s">
         <v>127</v>
       </c>
       <c r="F112" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="G112" s="54" t="s">
+      <c r="G112" s="52" t="s">
         <v>128</v>
       </c>
       <c r="H112" s="15" t="s">
@@ -6317,25 +6349,25 @@
       </c>
     </row>
     <row r="113" spans="1:8" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A113" s="45" t="s">
+      <c r="A113" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B113" s="83" t="s">
+      <c r="B113" s="81" t="s">
         <v>125</v>
       </c>
-      <c r="C113" s="61" t="s">
+      <c r="C113" s="59" t="s">
         <v>129</v>
       </c>
       <c r="D113" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="E113" s="54" t="s">
+      <c r="E113" s="52" t="s">
         <v>130</v>
       </c>
       <c r="F113" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="G113" s="54" t="s">
+      <c r="G113" s="52" t="s">
         <v>131</v>
       </c>
       <c r="H113" s="15" t="s">
@@ -6343,89 +6375,89 @@
       </c>
     </row>
     <row r="114" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A114" s="45" t="s">
+      <c r="A114" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B114" s="83"/>
-      <c r="C114" s="111" t="s">
-        <v>329</v>
-      </c>
-      <c r="D114" s="111"/>
-      <c r="E114" s="111"/>
-      <c r="F114" s="111"/>
-      <c r="G114" s="111"/>
-      <c r="H114" s="111"/>
+      <c r="B114" s="81"/>
+      <c r="C114" s="101" t="s">
+        <v>328</v>
+      </c>
+      <c r="D114" s="101"/>
+      <c r="E114" s="101"/>
+      <c r="F114" s="101"/>
+      <c r="G114" s="101"/>
+      <c r="H114" s="101"/>
     </row>
     <row r="115" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A115" s="49" t="s">
+      <c r="A115" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="B115" s="84"/>
-      <c r="C115" s="112" t="s">
-        <v>322</v>
-      </c>
-      <c r="D115" s="112"/>
-      <c r="E115" s="112"/>
-      <c r="F115" s="112"/>
-      <c r="G115" s="112"/>
-      <c r="H115" s="112"/>
+      <c r="B115" s="82"/>
+      <c r="C115" s="100" t="s">
+        <v>321</v>
+      </c>
+      <c r="D115" s="100"/>
+      <c r="E115" s="100"/>
+      <c r="F115" s="100"/>
+      <c r="G115" s="100"/>
+      <c r="H115" s="100"/>
     </row>
     <row r="116" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="100"/>
-      <c r="B116" s="100"/>
-      <c r="C116" s="100"/>
-      <c r="D116" s="100"/>
-      <c r="E116" s="100"/>
-      <c r="F116" s="100"/>
-      <c r="G116" s="100"/>
-      <c r="H116" s="100"/>
+      <c r="A116" s="102"/>
+      <c r="B116" s="102"/>
+      <c r="C116" s="102"/>
+      <c r="D116" s="102"/>
+      <c r="E116" s="102"/>
+      <c r="F116" s="102"/>
+      <c r="G116" s="102"/>
+      <c r="H116" s="102"/>
     </row>
     <row r="117" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="87" t="s">
+      <c r="A117" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="B117" s="44" t="s">
+      <c r="B117" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C117" s="113"/>
-      <c r="D117" s="113"/>
-      <c r="E117" s="113"/>
-      <c r="F117" s="113"/>
-      <c r="G117" s="113"/>
-      <c r="H117" s="113"/>
+      <c r="C117" s="99"/>
+      <c r="D117" s="99"/>
+      <c r="E117" s="99"/>
+      <c r="F117" s="99"/>
+      <c r="G117" s="99"/>
+      <c r="H117" s="99"/>
     </row>
     <row r="118" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A118" s="88" t="s">
+      <c r="A118" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="B118" s="89"/>
-      <c r="C118" s="111" t="s">
+      <c r="B118" s="87"/>
+      <c r="C118" s="101" t="s">
         <v>257</v>
       </c>
-      <c r="D118" s="111"/>
-      <c r="E118" s="111"/>
-      <c r="F118" s="111"/>
-      <c r="G118" s="111"/>
-      <c r="H118" s="111"/>
+      <c r="D118" s="101"/>
+      <c r="E118" s="101"/>
+      <c r="F118" s="101"/>
+      <c r="G118" s="101"/>
+      <c r="H118" s="101"/>
     </row>
     <row r="119" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A119" s="85" t="s">
+      <c r="A119" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="B119" s="89"/>
-      <c r="C119" s="61" t="s">
+      <c r="B119" s="87"/>
+      <c r="C119" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="D119" s="37" t="s">
+      <c r="D119" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="E119" s="54" t="s">
+      <c r="E119" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F119" s="37" t="s">
+      <c r="F119" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="G119" s="54" t="s">
+      <c r="G119" s="52" t="s">
         <v>138</v>
       </c>
       <c r="H119" s="23" t="s">
@@ -6433,25 +6465,25 @@
       </c>
     </row>
     <row r="120" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A120" s="45" t="s">
+      <c r="A120" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="B120" s="89" t="s">
+      <c r="B120" s="87" t="s">
         <v>140</v>
       </c>
-      <c r="C120" s="61" t="s">
+      <c r="C120" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="D120" s="37" t="s">
+      <c r="D120" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="E120" s="54" t="s">
+      <c r="E120" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="F120" s="37" t="s">
+      <c r="F120" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="G120" s="54" t="s">
+      <c r="G120" s="52" t="s">
         <v>143</v>
       </c>
       <c r="H120" s="23" t="s">
@@ -6459,97 +6491,211 @@
       </c>
     </row>
     <row r="121" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A121" s="76" t="s">
+      <c r="A121" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="B121" s="77"/>
-      <c r="C121" s="112" t="s">
+      <c r="B121" s="75"/>
+      <c r="C121" s="100" t="s">
         <v>257</v>
       </c>
-      <c r="D121" s="112"/>
-      <c r="E121" s="112"/>
-      <c r="F121" s="112"/>
-      <c r="G121" s="112"/>
-      <c r="H121" s="112"/>
+      <c r="D121" s="100"/>
+      <c r="E121" s="100"/>
+      <c r="F121" s="100"/>
+      <c r="G121" s="100"/>
+      <c r="H121" s="100"/>
     </row>
     <row r="122" spans="1:8" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="100"/>
-      <c r="B122" s="100"/>
-      <c r="C122" s="100"/>
-      <c r="D122" s="100"/>
-      <c r="E122" s="100"/>
-      <c r="F122" s="100"/>
-      <c r="G122" s="100"/>
-      <c r="H122" s="100"/>
+      <c r="A122" s="102"/>
+      <c r="B122" s="102"/>
+      <c r="C122" s="102"/>
+      <c r="D122" s="102"/>
+      <c r="E122" s="102"/>
+      <c r="F122" s="102"/>
+      <c r="G122" s="102"/>
+      <c r="H122" s="102"/>
     </row>
     <row r="123" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="43" t="s">
+      <c r="A123" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="B123" s="44" t="s">
+      <c r="B123" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="113"/>
-      <c r="D123" s="113"/>
-      <c r="E123" s="113"/>
-      <c r="F123" s="113"/>
-      <c r="G123" s="113"/>
-      <c r="H123" s="113"/>
+      <c r="C123" s="99"/>
+      <c r="D123" s="99"/>
+      <c r="E123" s="99"/>
+      <c r="F123" s="99"/>
+      <c r="G123" s="99"/>
+      <c r="H123" s="99"/>
     </row>
     <row r="124" spans="1:8" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A124" s="47" t="s">
+      <c r="A124" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="B124" s="90"/>
-      <c r="C124" s="111" t="s">
-        <v>323</v>
-      </c>
-      <c r="D124" s="111"/>
-      <c r="E124" s="111"/>
-      <c r="F124" s="111"/>
-      <c r="G124" s="111"/>
-      <c r="H124" s="111"/>
+      <c r="B124" s="88"/>
+      <c r="C124" s="101" t="s">
+        <v>322</v>
+      </c>
+      <c r="D124" s="101"/>
+      <c r="E124" s="101"/>
+      <c r="F124" s="101"/>
+      <c r="G124" s="101"/>
+      <c r="H124" s="101"/>
     </row>
     <row r="125" spans="1:8" s="2" customFormat="1" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="47" t="s">
+      <c r="A125" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="B125" s="90"/>
-      <c r="C125" s="125" t="s">
+      <c r="B125" s="88"/>
+      <c r="C125" s="104" t="s">
         <v>255</v>
       </c>
-      <c r="D125" s="125"/>
-      <c r="E125" s="125"/>
-      <c r="F125" s="125"/>
-      <c r="G125" s="125"/>
-      <c r="H125" s="125"/>
+      <c r="D125" s="104"/>
+      <c r="E125" s="104"/>
+      <c r="F125" s="104"/>
+      <c r="G125" s="104"/>
+      <c r="H125" s="104"/>
     </row>
     <row r="126" spans="1:8" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="49" t="s">
+      <c r="A126" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="B126" s="91"/>
-      <c r="C126" s="112"/>
-      <c r="D126" s="112"/>
-      <c r="E126" s="112"/>
-      <c r="F126" s="112"/>
-      <c r="G126" s="112"/>
-      <c r="H126" s="112"/>
+      <c r="B126" s="89"/>
+      <c r="C126" s="100"/>
+      <c r="D126" s="100"/>
+      <c r="E126" s="100"/>
+      <c r="F126" s="100"/>
+      <c r="G126" s="100"/>
+      <c r="H126" s="100"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="160">
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="C55:H55"/>
+    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="C49:H49"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="C61:H61"/>
+    <mergeCell ref="C62:H62"/>
+    <mergeCell ref="C63:H63"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="A57:H57"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="C59:H59"/>
+    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="C69:H69"/>
+    <mergeCell ref="C70:H70"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="C73:H73"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="C74:H74"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="A77:H77"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="A107:H107"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="C126:H126"/>
+    <mergeCell ref="C118:H118"/>
+    <mergeCell ref="C121:H121"/>
+    <mergeCell ref="A122:H122"/>
+    <mergeCell ref="C123:H123"/>
+    <mergeCell ref="C109:H109"/>
+    <mergeCell ref="C110:H110"/>
+    <mergeCell ref="C117:H117"/>
+    <mergeCell ref="C124:H124"/>
+    <mergeCell ref="D111:H111"/>
+    <mergeCell ref="C114:H114"/>
+    <mergeCell ref="C115:H115"/>
+    <mergeCell ref="A116:H116"/>
+    <mergeCell ref="C125:H125"/>
     <mergeCell ref="C95:E95"/>
     <mergeCell ref="F95:H95"/>
     <mergeCell ref="C96:E96"/>
@@ -6574,131 +6720,17 @@
     <mergeCell ref="C106:E106"/>
     <mergeCell ref="F106:H106"/>
     <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C126:H126"/>
-    <mergeCell ref="C118:H118"/>
-    <mergeCell ref="C121:H121"/>
-    <mergeCell ref="A122:H122"/>
-    <mergeCell ref="C123:H123"/>
-    <mergeCell ref="C109:H109"/>
-    <mergeCell ref="C110:H110"/>
-    <mergeCell ref="C117:H117"/>
-    <mergeCell ref="C124:H124"/>
-    <mergeCell ref="D111:H111"/>
-    <mergeCell ref="C114:H114"/>
-    <mergeCell ref="C115:H115"/>
-    <mergeCell ref="A116:H116"/>
-    <mergeCell ref="C125:H125"/>
-    <mergeCell ref="A77:H77"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="A107:H107"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="C73:H73"/>
-    <mergeCell ref="C65:H65"/>
-    <mergeCell ref="A66:H66"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="C74:H74"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="C61:H61"/>
-    <mergeCell ref="C62:H62"/>
-    <mergeCell ref="C63:H63"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="A57:H57"/>
-    <mergeCell ref="C58:H58"/>
-    <mergeCell ref="C59:H59"/>
-    <mergeCell ref="C60:H60"/>
-    <mergeCell ref="C69:H69"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="C53:H53"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="C55:H55"/>
-    <mergeCell ref="A56:H56"/>
-    <mergeCell ref="C49:H49"/>
-    <mergeCell ref="C50:H50"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="F99:H99"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -6748,169 +6780,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="90" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="90" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="90" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="90" t="s">
         <v>250</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="90" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="92" t="s">
+      <c r="H1" s="90" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="92" t="s">
+      <c r="I1" s="90" t="s">
         <v>251</v>
       </c>
-      <c r="J1" s="92" t="s">
+      <c r="J1" s="90" t="s">
         <v>211</v>
       </c>
-      <c r="K1" s="92" t="s">
+      <c r="K1" s="90" t="s">
         <v>212</v>
       </c>
-      <c r="L1" s="92" t="s">
+      <c r="L1" s="90" t="s">
         <v>213</v>
       </c>
-      <c r="M1" s="92" t="s">
+      <c r="M1" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="N1" s="92" t="s">
+      <c r="N1" s="90" t="s">
         <v>215</v>
       </c>
-      <c r="O1" s="92" t="s">
+      <c r="O1" s="90" t="s">
         <v>216</v>
       </c>
-      <c r="P1" s="92" t="s">
+      <c r="P1" s="90" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="92" t="s">
+      <c r="Q1" s="90" t="s">
         <v>218</v>
       </c>
-      <c r="R1" s="92" t="s">
+      <c r="R1" s="90" t="s">
         <v>219</v>
       </c>
-      <c r="S1" s="92" t="s">
+      <c r="S1" s="90" t="s">
         <v>220</v>
       </c>
-      <c r="T1" s="92" t="s">
+      <c r="T1" s="90" t="s">
         <v>240</v>
       </c>
-      <c r="U1" s="92" t="s">
+      <c r="U1" s="90" t="s">
         <v>241</v>
       </c>
-      <c r="V1" s="92" t="s">
+      <c r="V1" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="W1" s="92" t="s">
+      <c r="W1" s="90" t="s">
         <v>222</v>
       </c>
-      <c r="X1" s="92" t="s">
+      <c r="X1" s="90" t="s">
         <v>223</v>
       </c>
-      <c r="Y1" s="92" t="s">
+      <c r="Y1" s="90" t="s">
         <v>224</v>
       </c>
-      <c r="Z1" s="92" t="s">
+      <c r="Z1" s="90" t="s">
         <v>225</v>
       </c>
-      <c r="AA1" s="92" t="s">
+      <c r="AA1" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="AB1" s="92" t="s">
+      <c r="AB1" s="90" t="s">
         <v>242</v>
       </c>
-      <c r="AC1" s="92" t="s">
+      <c r="AC1" s="90" t="s">
         <v>243</v>
       </c>
-      <c r="AD1" s="92" t="s">
+      <c r="AD1" s="90" t="s">
         <v>227</v>
       </c>
-      <c r="AE1" s="92" t="s">
+      <c r="AE1" s="90" t="s">
         <v>244</v>
       </c>
-      <c r="AF1" s="92" t="s">
+      <c r="AF1" s="90" t="s">
         <v>245</v>
       </c>
-      <c r="AG1" s="92" t="s">
+      <c r="AG1" s="90" t="s">
         <v>228</v>
       </c>
-      <c r="AH1" s="92" t="s">
+      <c r="AH1" s="90" t="s">
         <v>229</v>
       </c>
-      <c r="AI1" s="92" t="s">
+      <c r="AI1" s="90" t="s">
         <v>230</v>
       </c>
-      <c r="AJ1" s="92" t="s">
+      <c r="AJ1" s="90" t="s">
         <v>231</v>
       </c>
-      <c r="AK1" s="92" t="s">
+      <c r="AK1" s="90" t="s">
         <v>232</v>
       </c>
-      <c r="AL1" s="92" t="s">
+      <c r="AL1" s="90" t="s">
         <v>233</v>
       </c>
-      <c r="AM1" s="92" t="s">
+      <c r="AM1" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="AN1" s="92" t="s">
+      <c r="AN1" s="90" t="s">
         <v>246</v>
       </c>
-      <c r="AO1" s="92" t="s">
+      <c r="AO1" s="90" t="s">
         <v>247</v>
       </c>
-      <c r="AP1" s="92" t="s">
+      <c r="AP1" s="90" t="s">
         <v>248</v>
       </c>
-      <c r="AQ1" s="92" t="s">
+      <c r="AQ1" s="90" t="s">
         <v>249</v>
       </c>
-      <c r="AR1" s="92" t="s">
+      <c r="AR1" s="90" t="s">
         <v>235</v>
       </c>
-      <c r="AS1" s="92" t="s">
+      <c r="AS1" s="90" t="s">
         <v>236</v>
       </c>
-      <c r="AT1" s="92" t="s">
+      <c r="AT1" s="90" t="s">
         <v>237</v>
       </c>
-      <c r="AU1" s="92" t="s">
+      <c r="AU1" s="90" t="s">
         <v>238</v>
       </c>
-      <c r="AV1" s="92" t="s">
+      <c r="AV1" s="90" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A2" s="93">
+      <c r="A2" s="91">
         <f>FS_Specs_EV!C3</f>
         <v>281</v>
       </c>
-      <c r="B2" s="93">
+      <c r="B2" s="91">
         <f>FS_Specs_EV!D7</f>
         <v>2757</v>
       </c>
-      <c r="C2" s="93">
+      <c r="C2" s="91">
         <f>FS_Specs_EV!F7</f>
         <v>1460</v>
       </c>
-      <c r="D2" s="93">
+      <c r="D2" s="91">
         <f>FS_Specs_EV!H7</f>
         <v>1272</v>
       </c>
-      <c r="E2" s="93">
+      <c r="E2" s="91">
         <f>FS_Specs_EV!D8</f>
         <v>1605</v>
       </c>
@@ -6918,11 +6950,11 @@
         <f>CONCATENATE(B2,"/",C2,"/",D2,"/",E2)</f>
         <v>2757/1460/1272/1605</v>
       </c>
-      <c r="G2" s="93">
+      <c r="G2" s="91">
         <f>FS_Specs_EV!F8</f>
         <v>1254</v>
       </c>
-      <c r="H2" s="93">
+      <c r="H2" s="91">
         <f>FS_Specs_EV!H8</f>
         <v>1200</v>
       </c>
@@ -6930,15 +6962,15 @@
         <f>CONCATENATE(G2,"/",H2)</f>
         <v>1254/1200</v>
       </c>
-      <c r="J2" s="93">
+      <c r="J2" s="91">
         <f>FS_Specs_EV!H10</f>
         <v>230</v>
       </c>
-      <c r="K2" s="93">
+      <c r="K2" s="91">
         <f>FS_Specs_EV!D10</f>
         <v>101.2</v>
       </c>
-      <c r="L2" s="93">
+      <c r="L2" s="91">
         <f>FS_Specs_EV!F10</f>
         <v>128.80000000000001</v>
       </c>
@@ -6946,11 +6978,11 @@
         <f>CONCATENATE(K2,"/",L2)</f>
         <v>101,2/128,8</v>
       </c>
-      <c r="N2" s="93" t="str">
+      <c r="N2" s="91" t="str">
         <f>FS_Specs_EV!C16</f>
         <v>Double wishbone, rocker arm damper, pull-rod</v>
       </c>
-      <c r="O2" s="93" t="str">
+      <c r="O2" s="91" t="str">
         <f>FS_Specs_EV!F16</f>
         <v>Double wishbone, rocker arm damper, push-rod</v>
       </c>
@@ -6958,11 +6990,11 @@
         <f>CONCATENATE(N2," ","front","/",O2," ", "rear")</f>
         <v>Double wishbone, rocker arm damper, pull-rod front/Double wishbone, rocker arm damper, push-rod rear</v>
       </c>
-      <c r="Q2" s="93" t="str">
+      <c r="Q2" s="91" t="str">
         <f>FS_Specs_EV!C14</f>
         <v>205/470 R13 FORMULA STUDENT C19</v>
       </c>
-      <c r="R2" s="93" t="str">
+      <c r="R2" s="91" t="str">
         <f>FS_Specs_EV!F14</f>
         <v>205/470 R13 FORMULA STUDENT C19</v>
       </c>
@@ -6970,13 +7002,13 @@
         <f>CONCATENATE(Q2," ","front","/",R2," ","rear")</f>
         <v>205/470 R13 FORMULA STUDENT C19 front/205/470 R13 FORMULA STUDENT C19 rear</v>
       </c>
-      <c r="T2" s="93" t="str">
+      <c r="T2" s="91" t="str">
         <f>FS_Specs_EV!C15</f>
         <v xml:space="preserve">7 in  
 7 in  
 </v>
       </c>
-      <c r="U2" s="93" t="str">
+      <c r="U2" s="91" t="str">
         <f>FS_Specs_EV!F15</f>
         <v xml:space="preserve">7 in  
 </v>
@@ -6988,11 +7020,11 @@
  front/7 in  
  rear</v>
       </c>
-      <c r="W2" s="93" t="str">
+      <c r="W2" s="91" t="str">
         <f>FS_Specs_EV!C40</f>
         <v>Beringer brakes, MC 127, proportioning with rear by a balancer bar</v>
       </c>
-      <c r="X2" s="93" t="str">
+      <c r="X2" s="91" t="str">
         <f>FS_Specs_EV!F40</f>
         <v>Beringer brakes, MC 127, D piston: 12.7 mm.
 Piston stroke : 20 mm.</v>
@@ -7002,16 +7034,16 @@
         <v>Beringer brakes, MC 127, proportioning with rear by a balancer bar front/Beringer brakes, MC 127, D piston: 12.7 mm.
 Piston stroke : 20 mm. rear</v>
       </c>
-      <c r="Z2" s="93" t="str">
+      <c r="Z2" s="91" t="str">
         <f>FS_Specs_EV!C68</f>
         <v>Steel spaceframe</v>
       </c>
-      <c r="AA2" s="93"/>
-      <c r="AB2" s="93" t="str">
+      <c r="AA2" s="91"/>
+      <c r="AB2" s="91" t="str">
         <f>FS_Specs_EV!C79</f>
         <v>N/A</v>
       </c>
-      <c r="AC2" s="93" t="str">
+      <c r="AC2" s="91" t="str">
         <f>FS_Specs_EV!F79</f>
         <v>Emrax 228 Medium Voltage and liquid cooling</v>
       </c>
@@ -7019,11 +7051,11 @@
         <f>CONCATENATE(AB2," ","front","/",AB2," ","rear")</f>
         <v>N/A front/N/A rear</v>
       </c>
-      <c r="AE2" s="93" t="str">
+      <c r="AE2" s="91" t="str">
         <f>FS_Specs_EV!C95</f>
         <v>N/A</v>
       </c>
-      <c r="AF2" s="93" t="str">
+      <c r="AF2" s="91" t="str">
         <f>FS_Specs_EV!F95</f>
         <v>Hong Kong Mingda Electric Power</v>
       </c>
@@ -7031,24 +7063,24 @@
         <f>CONCATENATE(AE2," ","front","/",AF2," ","rear")</f>
         <v>N/A front/Hong Kong Mingda Electric Power rear</v>
       </c>
-      <c r="AH2" s="93"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="93"/>
-      <c r="AK2" s="93"/>
-      <c r="AM2" s="93"/>
-      <c r="AN2" s="93" t="str">
+      <c r="AH2" s="91"/>
+      <c r="AI2" s="91"/>
+      <c r="AJ2" s="91"/>
+      <c r="AK2" s="91"/>
+      <c r="AM2" s="91"/>
+      <c r="AN2" s="91" t="str">
         <f>FS_Specs_EV!C88</f>
         <v>N/A</v>
       </c>
-      <c r="AO2" s="93" t="str">
+      <c r="AO2" s="91" t="str">
         <f>FS_Specs_EV!F88</f>
         <v>109 at 5500 RPM</v>
       </c>
-      <c r="AP2" s="93" t="str">
+      <c r="AP2" s="91" t="str">
         <f>FS_Specs_EV!C86</f>
         <v>N/A</v>
       </c>
-      <c r="AQ2" s="93" t="str">
+      <c r="AQ2" s="91" t="str">
         <f>FS_Specs_EV!F86</f>
         <v>230  for a few seconds</v>
       </c>
@@ -7056,19 +7088,19 @@
         <f>CONCATENATE(AN2," ","front",",",AO2," ","rear","/",AP2," ","front",",",AQ2," ","rear")</f>
         <v>N/A front,109 at 5500 RPM rear/N/A front,230  for a few seconds rear</v>
       </c>
-      <c r="AS2" s="93" t="str">
+      <c r="AS2" s="91" t="str">
         <f>FS_Specs_EV!C109</f>
         <v>Chain : CBR.900.RR '92/95 16X42 RK530GXW # (SC29,SC28). No gear box</v>
       </c>
-      <c r="AT2" s="93" t="str">
+      <c r="AT2" s="91" t="str">
         <f>FS_Specs_EV!C110</f>
         <v>Adjustable limited slip differential</v>
       </c>
-      <c r="AU2" s="93" t="str">
+      <c r="AU2" s="91" t="str">
         <f>FS_Specs_EV!C111</f>
         <v>3,23:1</v>
       </c>
-      <c r="AV2" s="93" t="str">
+      <c r="AV2" s="91" t="str">
         <f>FS_Specs_EV!C125</f>
         <v>E.g. Team EV from the University of Wattage will be aiming for a top 10 finish at this year's Formula Student competition for their most successful campaign to date.  Established in 2010, the team last enjoyed success in the 2019 competition with their highest placed finish of 11th overall and third best scoring EV team.  Since 2019, focus has been on improved aerodynamics and power to weight ratio.  As well as a top 10 finish, the team will target finishing Endurance with an improved efficiency score.  Team Leader, Flo Voltage, and the team would like to thank their sponsors xxxx, ssss and rrrrr as well as Faculty Advisor Dr. E. Lectric and the University of Wattage for their continued support of the Formula Student programme.</v>
       </c>
@@ -7098,64 +7130,64 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1" style="40" customWidth="1"/>
-    <col min="2" max="2" width="113.77734375" style="40" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="40"/>
+    <col min="1" max="1" width="1" style="38" customWidth="1"/>
+    <col min="2" max="2" width="113.77734375" style="38" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="38"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="40" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="40" t="s">
         <v>252</v>
       </c>
     </row>

</xml_diff>